<commit_message>
Actualización de diagrama e identificadores
</commit_message>
<xml_diff>
--- a/IdentificadoresSUMO.xlsx
+++ b/IdentificadoresSUMO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\10mo Ciclo\Redes Vehiculares\Proyecto Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E864F68A-3BAC-459B-90DB-54B9838B6955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E547793F-25B2-46EA-86F2-649602979104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31560" yWindow="2745" windowWidth="17250" windowHeight="8865" xr2:uid="{6BF47577-48E4-44DE-A1E1-B6B57020E13B}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{6BF47577-48E4-44DE-A1E1-B6B57020E13B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
   <si>
     <t>CLA1</t>
   </si>
@@ -187,6 +187,30 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>NUA2</t>
+  </si>
+  <si>
+    <t>NUA1</t>
+  </si>
+  <si>
+    <t>NUA3</t>
+  </si>
+  <si>
+    <t>PA2</t>
+  </si>
+  <si>
+    <t>PA3</t>
+  </si>
+  <si>
+    <t>PB1</t>
+  </si>
+  <si>
+    <t>PC1</t>
+  </si>
+  <si>
+    <t>399285450#0</t>
   </si>
 </sst>
 </file>
@@ -544,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3988B21A-352E-4468-BAA6-657080123048}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A35"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -855,6 +879,65 @@
         <v>303057278</v>
       </c>
     </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36">
+        <v>552654210</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38">
+        <v>48202933</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39">
+        <v>305214685</v>
+      </c>
+      <c r="C39">
+        <v>542435213</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40">
+        <v>542440756</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>56</v>
+      </c>
+      <c r="B41">
+        <v>542435213</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>57</v>
+      </c>
+      <c r="B42">
+        <v>542440756</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>